<commit_message>
Updates board to rev 3
Updates thematic
Updates bom
</commit_message>
<xml_diff>
--- a/board/electrospinner-pcb/electrospinner.xlsx
+++ b/board/electrospinner-pcb/electrospinner.xlsx
@@ -11,8 +11,8 @@
   </sheets>
   <definedNames>
     <definedName name="BoardQty">'electrospinner. '!$H$1</definedName>
-    <definedName name="global_part_data">'electrospinner. '!$A$5:$H$35</definedName>
-    <definedName name="mouser_part_data">'electrospinner. '!$I$5:$M$35</definedName>
+    <definedName name="global_part_data">'electrospinner. '!$A$5:$H$36</definedName>
+    <definedName name="mouser_part_data">'electrospinner. '!$I$5:$M$36</definedName>
     <definedName name="TotalCost">'electrospinner. '!$H$3</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -243,12 +243,12 @@
           <t>Qty/Price Breaks:
   Qty  -  Unit$  -  Ext$
 ================
-     1   $2.33      $2.33
-    10   $2.33     $23.30
-    50   $2.33    $116.50
-   100   $2.03    $203.00
-  1000   $1.74  $1,740.00
- 10000   $1.45 $14,500.00</t>
+     1   $2.95      $2.95
+    10   $2.95     $29.50
+    50   $2.95    $147.50
+   100   $2.95    $295.00
+  1000   $2.95  $2,950.00
+ 10000   $2.95 $29,500.00</t>
         </r>
       </text>
     </comment>
@@ -294,7 +294,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K10" authorId="0">
+    <comment ref="K11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -315,7 +315,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K11" authorId="0">
+    <comment ref="K12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -336,7 +336,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K12" authorId="0">
+    <comment ref="K13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -357,7 +357,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K13" authorId="0">
+    <comment ref="K14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -378,7 +378,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K14" authorId="0">
+    <comment ref="K15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -399,7 +399,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K18" authorId="0">
+    <comment ref="K19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -420,7 +420,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K22" authorId="0">
+    <comment ref="K23" authorId="0">
       <text>
         <r>
           <rPr>
@@ -441,7 +441,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K23" authorId="0">
+    <comment ref="K24" authorId="0">
       <text>
         <r>
           <rPr>
@@ -462,7 +462,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K24" authorId="0">
+    <comment ref="K25" authorId="0">
       <text>
         <r>
           <rPr>
@@ -483,7 +483,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K25" authorId="0">
+    <comment ref="K26" authorId="0">
       <text>
         <r>
           <rPr>
@@ -504,7 +504,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K26" authorId="0">
+    <comment ref="K27" authorId="0">
       <text>
         <r>
           <rPr>
@@ -525,7 +525,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K27" authorId="0">
+    <comment ref="K28" authorId="0">
       <text>
         <r>
           <rPr>
@@ -546,7 +546,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K29" authorId="0">
+    <comment ref="K30" authorId="0">
       <text>
         <r>
           <rPr>
@@ -567,7 +567,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K32" authorId="0">
+    <comment ref="K33" authorId="0">
       <text>
         <r>
           <rPr>
@@ -588,7 +588,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K33" authorId="0">
+    <comment ref="K34" authorId="0">
       <text>
         <r>
           <rPr>
@@ -609,7 +609,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K34" authorId="0">
+    <comment ref="K35" authorId="0">
       <text>
         <r>
           <rPr>
@@ -630,7 +630,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G37" authorId="0">
+    <comment ref="G38" authorId="0">
       <text>
         <r>
           <rPr>
@@ -643,7 +643,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J37" authorId="0">
+    <comment ref="J38" authorId="0">
       <text>
         <r>
           <rPr>
@@ -661,7 +661,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="146">
   <si>
     <t>Global Part Info</t>
   </si>
@@ -693,7 +693,7 @@
     <t>A1</t>
   </si>
   <si>
-    <t>A4988_Breakout</t>
+    <t>Pololu_Breakout_DRV8825</t>
   </si>
   <si>
     <t>Module:Pololu_Breakout-16_15.2x20.3mm</t>
@@ -702,7 +702,7 @@
     <t>Pololu</t>
   </si>
   <si>
-    <t>2128</t>
+    <t>2977</t>
   </si>
   <si>
     <t>Barrel_Jack1</t>
@@ -732,6 +732,9 @@
     <t>AS0805KKX7R9BB104</t>
   </si>
   <si>
+    <t>C11</t>
+  </si>
+  <si>
     <t>C2</t>
   </si>
   <si>
@@ -984,7 +987,7 @@
     <t>USB_B_Header1</t>
   </si>
   <si>
-    <t>USB_B_Header?</t>
+    <t>USB</t>
   </si>
   <si>
     <t>Connector_USB:USB_B_OST_USB-B1HSxx_Horizontal</t>
@@ -1008,7 +1011,7 @@
     <t>Prj date:</t>
   </si>
   <si>
-    <t>Mon 25 Mar 2019 07:53:54 PM EDT</t>
+    <t>Mon 08 Apr 2019 04:11:23 PM EDT</t>
   </si>
   <si>
     <t>Board Qty:</t>
@@ -1023,7 +1026,7 @@
     <t>$ date:</t>
   </si>
   <si>
-    <t>2019-03-25 20:02:17</t>
+    <t>2019-04-08 16:11:31</t>
   </si>
   <si>
     <t>Mouser</t>
@@ -1038,7 +1041,7 @@
     <t>Cat#</t>
   </si>
   <si>
-    <t>534-2128</t>
+    <t>485-2977</t>
   </si>
   <si>
     <t>474-PRT-00119</t>
@@ -1588,7 +1591,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M66"/>
+  <dimension ref="A1:M68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="8" ySplit="6" topLeftCell="I7" activePane="bottomRight" state="frozen"/>
@@ -1616,13 +1619,13 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H1" s="4">
         <v>100</v>
@@ -1630,13 +1633,13 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H2" s="5">
         <f>TotalCost/BoardQty</f>
@@ -1645,33 +1648,33 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H3" s="6">
-        <f>SUM(H7:H35)</f>
+        <f>SUM(H7:H36)</f>
         <v>0</v>
       </c>
       <c r="L3" s="6">
-        <f>SUM(L7:L35)</f>
+        <f>SUM(L7:L36)</f>
         <v>0</v>
       </c>
       <c r="M3" s="7">
-        <f>(ROWS(L7:L35)-COUNTBLANK(L7:L35))&amp;" of "&amp;ROWS(L7:L35)&amp;" parts found"</f>
+        <f>(ROWS(L7:L36)-COUNTBLANK(L7:L36))&amp;" of "&amp;ROWS(L7:L36)&amp;" parts found"</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1686,7 +1689,7 @@
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
@@ -1719,10 +1722,10 @@
         <v>8</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="K6" s="10" t="s">
         <v>7</v>
@@ -1731,7 +1734,7 @@
         <v>8</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1763,10 +1766,10 @@
         <v>0</v>
       </c>
       <c r="I7" s="11">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="K7" s="12">
-        <f>iferror(lookup(if(J7="",F7,J7),{0,1,10,50,100,1000,10000},{0.0,2.33,2.33,2.33,2.03,1.7400000000000002,1.45}),"")</f>
+        <f>iferror(lookup(if(J7="",F7,J7),{0,1,10,50,100,1000,10000},{0.0,2.95,2.95,2.95,2.95,2.95,2.95}),"")</f>
         <v>0</v>
       </c>
       <c r="L7" s="12">
@@ -1774,7 +1777,7 @@
         <v>0</v>
       </c>
       <c r="M7" s="13" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -1803,7 +1806,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="11">
-        <v>1149</v>
+        <v>1106</v>
       </c>
       <c r="K8" s="12">
         <f>iferror(lookup(if(J8="",F8,J8),{0,1,10,50,100,1000,10000},{0.0,1.25,1.25,1.25,1.25,1.25,1.25}),"")</f>
@@ -1814,7 +1817,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="13" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -1846,7 +1849,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="11">
-        <v>25282</v>
+        <v>24156</v>
       </c>
       <c r="K9" s="12">
         <f>iferror(lookup(if(J9="",F9,J9),{0,1,10,50,100,1000,10000},{0.0,0.67,0.461,0.461,0.262,0.165,0.136}),"")</f>
@@ -1857,7 +1860,7 @@
         <v>0</v>
       </c>
       <c r="M9" s="13" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -1865,13 +1868,7 @@
         <v>23</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F10" s="11">
         <f>BoardQty*1</f>
@@ -1885,36 +1882,19 @@
         <f>iferror(F10*G10,"")</f>
         <v>0</v>
       </c>
-      <c r="I10" s="11">
-        <v>26517</v>
-      </c>
-      <c r="K10" s="12">
-        <f>iferror(lookup(if(J10="",F10,J10),{0,1,10,50,100,1000,10000},{0.0,1.06,0.75,0.75,0.473,0.388,0.24700000000000003}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="L10" s="12">
-        <f>iferror(if(J10="",F10,J10)*K10,"")</f>
-        <v>0</v>
-      </c>
-      <c r="M10" s="13" t="s">
-        <v>128</v>
-      </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>30</v>
       </c>
       <c r="F11" s="11">
         <f>BoardQty*1</f>
@@ -1929,10 +1909,10 @@
         <v>0</v>
       </c>
       <c r="I11" s="11">
-        <v>3811</v>
+        <v>35924</v>
       </c>
       <c r="K11" s="12">
-        <f>iferror(lookup(if(J11="",F11,J11),{0,1,10,50,100,1000,10000},{0.0,0.6000000000000001,0.483,0.483,0.276,0.174,0.143}),"")</f>
+        <f>iferror(lookup(if(J11="",F11,J11),{0,1,10,50,100,1000,10000},{0.0,1.06,0.75,0.75,0.473,0.388,0.24700000000000003}),"")</f>
         <v>0</v>
       </c>
       <c r="L11" s="12">
@@ -1945,16 +1925,19 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>31</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>33</v>
       </c>
       <c r="F12" s="11">
         <f>BoardQty*1</f>
@@ -1969,10 +1952,10 @@
         <v>0</v>
       </c>
       <c r="I12" s="11">
-        <v>2744</v>
+        <v>3769</v>
       </c>
       <c r="K12" s="12">
-        <f>iferror(lookup(if(J12="",F12,J12),{0,1,10,50,100,1000,10000},{0.0,0.59,0.344,0.344,0.233,0.194,0.11899999999999998}),"")</f>
+        <f>iferror(lookup(if(J12="",F12,J12),{0,1,10,50,100,1000,10000},{0.0,0.6000000000000001,0.483,0.483,0.276,0.174,0.143}),"")</f>
         <v>0</v>
       </c>
       <c r="L12" s="12">
@@ -1985,22 +1968,19 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>37</v>
-      </c>
       <c r="F13" s="11">
-        <f>BoardQty*5</f>
+        <f>BoardQty*1</f>
         <v>0</v>
       </c>
       <c r="G13" s="12">
@@ -2012,10 +1992,10 @@
         <v>0</v>
       </c>
       <c r="I13" s="11">
-        <v>393604</v>
+        <v>2644</v>
       </c>
       <c r="K13" s="12">
-        <f>iferror(lookup(if(J13="",F13,J13),{0,1,10,50,100,1000,10000},{0.0,0.24,0.113,0.113,0.076,0.062,0.042}),"")</f>
+        <f>iferror(lookup(if(J13="",F13,J13),{0,1,10,50,100,1000,10000},{0.0,0.59,0.344,0.344,0.233,0.194,0.11899999999999998}),"")</f>
         <v>0</v>
       </c>
       <c r="L13" s="12">
@@ -2028,19 +2008,22 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>40</v>
-      </c>
       <c r="F14" s="11">
-        <f>BoardQty*1</f>
+        <f>BoardQty*5</f>
         <v>0</v>
       </c>
       <c r="G14" s="12">
@@ -2052,10 +2035,10 @@
         <v>0</v>
       </c>
       <c r="I14" s="11">
-        <v>10161</v>
+        <v>378604</v>
       </c>
       <c r="K14" s="12">
-        <f>iferror(lookup(if(J14="",F14,J14),{0,1,10,50,100,1000,10000},{0.0,0.38,0.264,0.264,0.15000000000000002,0.092,0.069}),"")</f>
+        <f>iferror(lookup(if(J14="",F14,J14),{0,1,10,50,100,1000,10000},{0.0,0.24,0.113,0.113,0.076,0.062,0.042}),"")</f>
         <v>0</v>
       </c>
       <c r="L14" s="12">
@@ -2068,13 +2051,16 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="F15" s="11">
         <f>BoardQty*1</f>
@@ -2088,16 +2074,30 @@
         <f>iferror(F15*G15,"")</f>
         <v>0</v>
       </c>
+      <c r="I15" s="11">
+        <v>6838</v>
+      </c>
+      <c r="K15" s="12">
+        <f>iferror(lookup(if(J15="",F15,J15),{0,1,10,50,100,1000,10000},{0.0,0.38,0.264,0.264,0.15000000000000002,0.092,0.069}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="L15" s="12">
+        <f>iferror(if(J15="",F15,J15)*K15,"")</f>
+        <v>0</v>
+      </c>
+      <c r="M15" s="13" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>44</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="F16" s="11">
         <f>BoardQty*1</f>
@@ -2114,13 +2114,13 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="11" t="s">
-        <v>47</v>
-      </c>
       <c r="C17" s="11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F17" s="11">
         <f>BoardQty*1</f>
@@ -2137,16 +2137,13 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>49</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>52</v>
       </c>
       <c r="F18" s="11">
         <f>BoardQty*1</f>
@@ -2160,30 +2157,19 @@
         <f>iferror(F18*G18,"")</f>
         <v>0</v>
       </c>
-      <c r="I18" s="11">
-        <v>5160</v>
-      </c>
-      <c r="K18" s="12">
-        <f>iferror(lookup(if(J18="",F18,J18),{0,1,10,50,100,1000,10000},{0.0,0.73,0.637,0.637,0.45400000000000007,0.269,0.237}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="L18" s="12">
-        <f>iferror(if(J18="",F18,J18)*K18,"")</f>
-        <v>0</v>
-      </c>
-      <c r="M18" s="13" t="s">
-        <v>133</v>
-      </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="11" t="s">
         <v>53</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>55</v>
       </c>
       <c r="F19" s="11">
         <f>BoardQty*1</f>
@@ -2197,13 +2183,30 @@
         <f>iferror(F19*G19,"")</f>
         <v>0</v>
       </c>
+      <c r="I19" s="11">
+        <v>5135</v>
+      </c>
+      <c r="K19" s="12">
+        <f>iferror(lookup(if(J19="",F19,J19),{0,1,10,50,100,1000,10000},{0.0,0.73,0.637,0.637,0.45400000000000007,0.269,0.237}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="L19" s="12">
+        <f>iferror(if(J19="",F19,J19)*K19,"")</f>
+        <v>0</v>
+      </c>
+      <c r="M19" s="13" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>56</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>57</v>
       </c>
       <c r="F20" s="11">
         <f>BoardQty*1</f>
@@ -2220,16 +2223,10 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="11" t="s">
         <v>58</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>61</v>
       </c>
       <c r="F21" s="11">
         <f>BoardQty*1</f>
@@ -2246,19 +2243,16 @@
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="11" t="s">
         <v>62</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>66</v>
       </c>
       <c r="F22" s="11">
         <f>BoardQty*1</f>
@@ -2272,36 +2266,22 @@
         <f>iferror(F22*G22,"")</f>
         <v>0</v>
       </c>
-      <c r="I22" s="11">
-        <v>113570</v>
-      </c>
-      <c r="K22" s="12">
-        <f>iferror(lookup(if(J22="",F22,J22),{0,1,10,50,100,1000,10000},{0.0,0.1,0.031,0.031,0.017,0.009999999999999998,0.007}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="L22" s="12">
-        <f>iferror(if(J22="",F22,J22)*K22,"")</f>
-        <v>0</v>
-      </c>
-      <c r="M22" s="13" t="s">
-        <v>134</v>
-      </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="11" t="s">
         <v>67</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>71</v>
       </c>
       <c r="F23" s="11">
         <f>BoardQty*1</f>
@@ -2316,10 +2296,10 @@
         <v>0</v>
       </c>
       <c r="I23" s="11">
-        <v>14679</v>
+        <v>113570</v>
       </c>
       <c r="K23" s="12">
-        <f>iferror(lookup(if(J23="",F23,J23),{0,1,10,50,100,1000,10000},{0.0,0.23,0.23,0.17900000000000002,0.154,0.115,0.085}),"")</f>
+        <f>iferror(lookup(if(J23="",F23,J23),{0,1,10,50,100,1000,10000},{0.0,0.1,0.031,0.031,0.017,0.009999999999999998,0.007}),"")</f>
         <v>0</v>
       </c>
       <c r="L23" s="12">
@@ -2332,16 +2312,19 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" s="11" t="s">
         <v>72</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>74</v>
       </c>
       <c r="F24" s="11">
         <f>BoardQty*1</f>
@@ -2356,10 +2339,10 @@
         <v>0</v>
       </c>
       <c r="I24" s="11">
-        <v>9461</v>
+        <v>14531</v>
       </c>
       <c r="K24" s="12">
-        <f>iferror(lookup(if(J24="",F24,J24),{0,1,10,50,100,1000,10000},{0.0,0.14,0.077,0.064,0.043,0.019999999999999997,0.019999999999999997}),"")</f>
+        <f>iferror(lookup(if(J24="",F24,J24),{0,1,10,50,100,1000,10000},{0.0,0.23,0.23,0.17900000000000002,0.154,0.115,0.085}),"")</f>
         <v>0</v>
       </c>
       <c r="L24" s="12">
@@ -2372,16 +2355,16 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="11" t="s">
         <v>75</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>77</v>
       </c>
       <c r="F25" s="11">
         <f>BoardQty*1</f>
@@ -2396,10 +2379,10 @@
         <v>0</v>
       </c>
       <c r="I25" s="11">
-        <v>57571</v>
+        <v>9459</v>
       </c>
       <c r="K25" s="12">
-        <f>iferror(lookup(if(J25="",F25,J25),{0,1,10,50,100,1000,10000},{0.0,0.14,0.065,0.065,0.035,0.012,0.006}),"")</f>
+        <f>iferror(lookup(if(J25="",F25,J25),{0,1,10,50,100,1000,10000},{0.0,0.14,0.077,0.064,0.043,0.019999999999999997,0.019999999999999997}),"")</f>
         <v>0</v>
       </c>
       <c r="L25" s="12">
@@ -2412,19 +2395,19 @@
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="B26" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>80</v>
-      </c>
       <c r="F26" s="11">
-        <f>BoardQty*2</f>
+        <f>BoardQty*1</f>
         <v>0</v>
       </c>
       <c r="G26" s="12">
@@ -2436,10 +2419,10 @@
         <v>0</v>
       </c>
       <c r="I26" s="11">
-        <v>9584</v>
+        <v>57541</v>
       </c>
       <c r="K26" s="12">
-        <f>iferror(lookup(if(J26="",F26,J26),{0,1,10,50,100,1000,10000},{0.0,0.14,0.077,0.064,0.043,0.019999999999999997,0.019999999999999997}),"")</f>
+        <f>iferror(lookup(if(J26="",F26,J26),{0,1,10,50,100,1000,10000},{0.0,0.14,0.065,0.065,0.035,0.012,0.006}),"")</f>
         <v>0</v>
       </c>
       <c r="L26" s="12">
@@ -2452,19 +2435,19 @@
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="B27" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>83</v>
-      </c>
       <c r="F27" s="11">
-        <f>BoardQty*1</f>
+        <f>BoardQty*2</f>
         <v>0</v>
       </c>
       <c r="G27" s="12">
@@ -2476,10 +2459,10 @@
         <v>0</v>
       </c>
       <c r="I27" s="11">
-        <v>5605</v>
+        <v>9584</v>
       </c>
       <c r="K27" s="12">
-        <f>iferror(lookup(if(J27="",F27,J27),{0,1,10,50,100,1000,10000},{0.0,0.23,0.23,0.17900000000000002,0.154,0.115,0.085}),"")</f>
+        <f>iferror(lookup(if(J27="",F27,J27),{0,1,10,50,100,1000,10000},{0.0,0.14,0.077,0.064,0.043,0.019999999999999997,0.019999999999999997}),"")</f>
         <v>0</v>
       </c>
       <c r="L27" s="12">
@@ -2492,13 +2475,16 @@
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E28" s="11" t="s">
         <v>84</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>86</v>
       </c>
       <c r="F28" s="11">
         <f>BoardQty*1</f>
@@ -2512,19 +2498,30 @@
         <f>iferror(F28*G28,"")</f>
         <v>0</v>
       </c>
+      <c r="I28" s="11">
+        <v>5375</v>
+      </c>
+      <c r="K28" s="12">
+        <f>iferror(lookup(if(J28="",F28,J28),{0,1,10,50,100,1000,10000},{0.0,0.23,0.23,0.17900000000000002,0.154,0.115,0.085}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="L28" s="12">
+        <f>iferror(if(J28="",F28,J28)*K28,"")</f>
+        <v>0</v>
+      </c>
+      <c r="M28" s="13" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="11" t="s">
         <v>87</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>89</v>
       </c>
       <c r="F29" s="11">
         <f>BoardQty*1</f>
@@ -2538,30 +2535,19 @@
         <f>iferror(F29*G29,"")</f>
         <v>0</v>
       </c>
-      <c r="I29" s="11">
-        <v>20072</v>
-      </c>
-      <c r="K29" s="12">
-        <f>iferror(lookup(if(J29="",F29,J29),{0,1,10,50,100,1000,10000},{0.0,0.35,0.334,0.242,0.233,0.166,0.143}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="L29" s="12">
-        <f>iferror(if(J29="",F29,J29)*K29,"")</f>
-        <v>0</v>
-      </c>
-      <c r="M29" s="13" t="s">
-        <v>140</v>
-      </c>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="11" t="s">
         <v>90</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>92</v>
       </c>
       <c r="F30" s="11">
         <f>BoardQty*1</f>
@@ -2575,13 +2561,30 @@
         <f>iferror(F30*G30,"")</f>
         <v>0</v>
       </c>
+      <c r="I30" s="11">
+        <v>26048</v>
+      </c>
+      <c r="K30" s="12">
+        <f>iferror(lookup(if(J30="",F30,J30),{0,1,10,50,100,1000,10000},{0.0,0.35,0.334,0.242,0.233,0.166,0.143}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="L30" s="12">
+        <f>iferror(if(J30="",F30,J30)*K30,"")</f>
+        <v>0</v>
+      </c>
+      <c r="M30" s="13" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="11" t="s">
         <v>93</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>94</v>
       </c>
       <c r="F31" s="11">
         <f>BoardQty*1</f>
@@ -2598,16 +2601,10 @@
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32" s="11" t="s">
         <v>95</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>98</v>
       </c>
       <c r="F32" s="11">
         <f>BoardQty*1</f>
@@ -2621,33 +2618,19 @@
         <f>iferror(F32*G32,"")</f>
         <v>0</v>
       </c>
-      <c r="I32" s="11">
-        <v>110049</v>
-      </c>
-      <c r="K32" s="12">
-        <f>iferror(lookup(if(J32="",F32,J32),{0,1,10,50,100,1000,10000},{0.0,2.04,2.04,1.97,1.9000000000000001,1.46,1.4}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="L32" s="12">
-        <f>iferror(if(J32="",F32,J32)*K32,"")</f>
-        <v>0</v>
-      </c>
-      <c r="M32" s="13" t="s">
-        <v>141</v>
-      </c>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="E33" s="11" t="s">
         <v>99</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>102</v>
       </c>
       <c r="F33" s="11">
         <f>BoardQty*1</f>
@@ -2662,10 +2645,10 @@
         <v>0</v>
       </c>
       <c r="I33" s="11">
-        <v>26564</v>
+        <v>106176</v>
       </c>
       <c r="K33" s="12">
-        <f>iferror(lookup(if(J33="",F33,J33),{0,1,10,50,100,1000,10000},{0.0,2.15,1.83,1.83,1.46,1.06,0.949}),"")</f>
+        <f>iferror(lookup(if(J33="",F33,J33),{0,1,10,50,100,1000,10000},{0.0,2.04,2.04,1.97,1.9000000000000001,1.46,1.4}),"")</f>
         <v>0</v>
       </c>
       <c r="L33" s="12">
@@ -2678,16 +2661,16 @@
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E34" s="11" t="s">
         <v>103</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>104</v>
       </c>
       <c r="F34" s="11">
         <f>BoardQty*1</f>
@@ -2702,10 +2685,10 @@
         <v>0</v>
       </c>
       <c r="I34" s="11">
-        <v>1871</v>
+        <v>26496</v>
       </c>
       <c r="K34" s="12">
-        <f>iferror(lookup(if(J34="",F34,J34),{0,1,10,50,100,1000,10000},{0.0,2.46,2.09,2.09,1.68,1.22,1.09}),"")</f>
+        <f>iferror(lookup(if(J34="",F34,J34),{0,1,10,50,100,1000,10000},{0.0,2.15,1.83,1.83,1.46,1.06,0.949}),"")</f>
         <v>0</v>
       </c>
       <c r="L34" s="12">
@@ -2718,13 +2701,16 @@
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="B35" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>108</v>
+      <c r="E35" s="11" t="s">
+        <v>105</v>
       </c>
       <c r="F35" s="11">
         <f>BoardQty*1</f>
@@ -2738,430 +2724,481 @@
         <f>iferror(F35*G35,"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="A37" s="3" t="s">
+      <c r="I35" s="11">
+        <v>1771</v>
+      </c>
+      <c r="K35" s="12">
+        <f>iferror(lookup(if(J35="",F35,J35),{0,1,10,50,100,1000,10000},{0.0,2.46,2.09,2.09,1.68,1.22,1.09}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="L35" s="12">
+        <f>iferror(if(J35="",F35,J35)*K35,"")</f>
+        <v>0</v>
+      </c>
+      <c r="M35" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="G37" s="2" t="s">
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C36" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="H37" s="6">
+      <c r="F36" s="11">
+        <f>BoardQty*1</f>
+        <v>0</v>
+      </c>
+      <c r="G36" s="12">
+        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
+        <v>0</v>
+      </c>
+      <c r="H36" s="12">
+        <f>iferror(F36*G36,"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H38" s="6">
         <f>SUM(INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+3)))</f>
         <v>0</v>
       </c>
-      <c r="J37" s="7">
-        <f>IFERROR(IF(OR(J7:J35),COUNTIFS(J7:J35,"&gt;0",L7:L35,"&lt;&gt;")&amp;" of "&amp;(ROWS(L7:L35)-COUNTBLANK(L7:L35))&amp;" parts purchased",""),"")</f>
-        <v>0</v>
-      </c>
-      <c r="L37" s="6">
-        <f>SUMIF(J7:J35,"&gt;0",L7:L35)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13">
-      <c r="J38">
-        <f t="array" ref="J38">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
-        <v>0</v>
-      </c>
-      <c r="K38">
-        <f t="array" ref="K38">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
-        <v>0</v>
-      </c>
-      <c r="L38">
-        <f t="array" ref="L38">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
+      <c r="J38" s="7">
+        <f>IFERROR(IF(OR(J7:J36),COUNTIFS(J7:J36,"&gt;0",L7:L36,"&lt;&gt;")&amp;" of "&amp;(ROWS(L7:L36)-COUNTBLANK(L7:L36))&amp;" parts purchased",""),"")</f>
+        <v>0</v>
+      </c>
+      <c r="L38" s="6">
+        <f>SUMIF(J7:J36,"&gt;0",L7:L36)</f>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:13">
       <c r="J39">
-        <f t="array" ref="J39">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
+        <f t="array" ref="J39">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K39">
-        <f t="array" ref="K39">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K39">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L39">
-        <f t="array" ref="L39">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
+        <f t="array" ref="L39">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:13">
       <c r="J40">
-        <f t="array" ref="J40">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
+        <f t="array" ref="J40">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K40">
-        <f t="array" ref="K40">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K40">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L40">
-        <f t="array" ref="L40">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
+        <f t="array" ref="L40">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:13">
       <c r="J41">
-        <f t="array" ref="J41">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
+        <f t="array" ref="J41">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K41">
-        <f t="array" ref="K41">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K41">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L41">
-        <f t="array" ref="L41">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
+        <f t="array" ref="L41">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:13">
       <c r="J42">
-        <f t="array" ref="J42">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
+        <f t="array" ref="J42">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K42">
-        <f t="array" ref="K42">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K42">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L42">
-        <f t="array" ref="L42">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
+        <f t="array" ref="L42">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:13">
       <c r="J43">
-        <f t="array" ref="J43">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
+        <f t="array" ref="J43">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K43">
-        <f t="array" ref="K43">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K43">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L43">
-        <f t="array" ref="L43">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
+        <f t="array" ref="L43">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:13">
       <c r="J44">
-        <f t="array" ref="J44">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
+        <f t="array" ref="J44">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K44">
-        <f t="array" ref="K44">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K44">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L44">
-        <f t="array" ref="L44">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
+        <f t="array" ref="L44">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:13">
       <c r="J45">
-        <f t="array" ref="J45">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
+        <f t="array" ref="J45">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K45">
-        <f t="array" ref="K45">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K45">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L45">
-        <f t="array" ref="L45">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
+        <f t="array" ref="L45">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:13">
       <c r="J46">
-        <f t="array" ref="J46">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
+        <f t="array" ref="J46">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K46">
-        <f t="array" ref="K46">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K46">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L46">
-        <f t="array" ref="L46">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
+        <f t="array" ref="L46">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:13">
       <c r="J47">
-        <f t="array" ref="J47">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
+        <f t="array" ref="J47">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K47">
-        <f t="array" ref="K47">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K47">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L47">
-        <f t="array" ref="L47">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
+        <f t="array" ref="L47">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:13">
       <c r="J48">
-        <f t="array" ref="J48">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
+        <f t="array" ref="J48">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K48">
-        <f t="array" ref="K48">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K48">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L48">
-        <f t="array" ref="L48">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
+        <f t="array" ref="L48">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="10:12">
       <c r="J49">
-        <f t="array" ref="J49">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
+        <f t="array" ref="J49">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K49">
-        <f t="array" ref="K49">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K49">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L49">
-        <f t="array" ref="L49">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
+        <f t="array" ref="L49">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="10:12">
       <c r="J50">
-        <f t="array" ref="J50">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
+        <f t="array" ref="J50">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K50">
-        <f t="array" ref="K50">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K50">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L50">
-        <f t="array" ref="L50">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
+        <f t="array" ref="L50">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="10:12">
       <c r="J51">
-        <f t="array" ref="J51">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
+        <f t="array" ref="J51">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K51">
-        <f t="array" ref="K51">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K51">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L51">
-        <f t="array" ref="L51">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
+        <f t="array" ref="L51">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="10:12">
       <c r="J52">
-        <f t="array" ref="J52">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
+        <f t="array" ref="J52">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K52">
-        <f t="array" ref="K52">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K52">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L52">
-        <f t="array" ref="L52">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
+        <f t="array" ref="L52">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="10:12">
       <c r="J53">
-        <f t="array" ref="J53">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
+        <f t="array" ref="J53">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K53">
-        <f t="array" ref="K53">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K53">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L53">
-        <f t="array" ref="L53">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
+        <f t="array" ref="L53">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="10:12">
       <c r="J54">
-        <f t="array" ref="J54">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
+        <f t="array" ref="J54">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K54">
-        <f t="array" ref="K54">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K54">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L54">
-        <f t="array" ref="L54">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
+        <f t="array" ref="L54">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="10:12">
       <c r="J55">
-        <f t="array" ref="J55">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
+        <f t="array" ref="J55">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K55">
-        <f t="array" ref="K55">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K55">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L55">
-        <f t="array" ref="L55">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
+        <f t="array" ref="L55">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="10:12">
       <c r="J56">
-        <f t="array" ref="J56">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
+        <f t="array" ref="J56">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K56">
-        <f t="array" ref="K56">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K56">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L56">
-        <f t="array" ref="L56">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
+        <f t="array" ref="L56">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="10:12">
       <c r="J57">
-        <f t="array" ref="J57">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
+        <f t="array" ref="J57">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K57">
-        <f t="array" ref="K57">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K57">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L57">
-        <f t="array" ref="L57">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
+        <f t="array" ref="L57">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="10:12">
       <c r="J58">
-        <f t="array" ref="J58">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
+        <f t="array" ref="J58">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K58">
-        <f t="array" ref="K58">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K58">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L58">
-        <f t="array" ref="L58">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
+        <f t="array" ref="L58">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="10:12">
       <c r="J59">
-        <f t="array" ref="J59">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
+        <f t="array" ref="J59">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K59">
-        <f t="array" ref="K59">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K59">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L59">
-        <f t="array" ref="L59">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
+        <f t="array" ref="L59">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="10:12">
       <c r="J60">
-        <f t="array" ref="J60">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
+        <f t="array" ref="J60">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K60">
-        <f t="array" ref="K60">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K60">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L60">
-        <f t="array" ref="L60">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
+        <f t="array" ref="L60">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="10:12">
       <c r="J61">
-        <f t="array" ref="J61">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
+        <f t="array" ref="J61">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K61">
-        <f t="array" ref="K61">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K61">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L61">
-        <f t="array" ref="L61">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
+        <f t="array" ref="L61">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="10:12">
       <c r="J62">
-        <f t="array" ref="J62">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
+        <f t="array" ref="J62">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K62">
-        <f t="array" ref="K62">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K62">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L62">
-        <f t="array" ref="L62">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
+        <f t="array" ref="L62">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="10:12">
       <c r="J63">
-        <f t="array" ref="J63">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
+        <f t="array" ref="J63">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K63">
-        <f t="array" ref="K63">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K63">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L63">
-        <f t="array" ref="L63">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
+        <f t="array" ref="L63">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="10:12">
       <c r="J64">
-        <f t="array" ref="J64">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
+        <f t="array" ref="J64">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K64">
-        <f t="array" ref="K64">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K64">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L64">
-        <f t="array" ref="L64">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
+        <f t="array" ref="L64">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="10:12">
       <c r="J65">
-        <f t="array" ref="J65">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
+        <f t="array" ref="J65">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K65">
-        <f t="array" ref="K65">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K65">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L65">
-        <f t="array" ref="L65">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
+        <f t="array" ref="L65">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="10:12">
       <c r="J66">
-        <f t="array" ref="J66">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
+        <f t="array" ref="J66">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K66">
-        <f t="array" ref="K66">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K66">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L66">
-        <f t="array" ref="L66">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
+        <f t="array" ref="L66">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="10:12">
+      <c r="J67">
+        <f t="array" ref="J67">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <v>0</v>
+      </c>
+      <c r="K67">
+        <f t="array" ref="K67">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <v>0</v>
+      </c>
+      <c r="L67">
+        <f t="array" ref="L67">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="10:12">
+      <c r="J68">
+        <f t="array" ref="J68">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <v>0</v>
+      </c>
+      <c r="K68">
+        <f t="array" ref="K68">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <v>0</v>
+      </c>
+      <c r="L68">
+        <f t="array" ref="L68">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
@@ -3534,6 +3571,20 @@
       <formula>SUM(IF(ISNUMBER(INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2))),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+1)),0))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F36">
+    <cfRule type="expression" dxfId="0" priority="117">
+      <formula>AND(ISBLANK(E36),ISBLANK(INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+4))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="118">
+      <formula>IF(SUM(INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+0)))=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="119" operator="greaterThan">
+      <formula>SUM(INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+0)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="120" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2))),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+1)),0))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F7">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND(ISBLANK(E7),ISBLANK(INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+4))))</formula>
@@ -3576,250 +3627,250 @@
       <formula>SUM(IF(ISNUMBER(INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2))),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+1)),0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I10">
-    <cfRule type="cellIs" dxfId="1" priority="126" operator="equal">
+  <conditionalFormatting sqref="I11">
+    <cfRule type="cellIs" dxfId="1" priority="130" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="127" operator="lessThan">
-      <formula>F10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I11">
-    <cfRule type="cellIs" dxfId="1" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="131" operator="lessThan">
+      <formula>F11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12">
+    <cfRule type="cellIs" dxfId="1" priority="133" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="130" operator="lessThan">
-      <formula>F11</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
-    <cfRule type="cellIs" dxfId="1" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="134" operator="lessThan">
+      <formula>F12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
+    <cfRule type="cellIs" dxfId="1" priority="136" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="133" operator="lessThan">
-      <formula>F12</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
-    <cfRule type="cellIs" dxfId="1" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="137" operator="lessThan">
+      <formula>F13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14">
+    <cfRule type="cellIs" dxfId="1" priority="139" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="136" operator="lessThan">
-      <formula>F13</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="1" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="140" operator="lessThan">
+      <formula>F14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15">
+    <cfRule type="cellIs" dxfId="1" priority="142" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="139" operator="lessThan">
-      <formula>F14</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18">
-    <cfRule type="cellIs" dxfId="1" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="143" operator="lessThan">
+      <formula>F15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I19">
+    <cfRule type="cellIs" dxfId="1" priority="145" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="142" operator="lessThan">
-      <formula>F18</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I22">
-    <cfRule type="cellIs" dxfId="1" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="146" operator="lessThan">
+      <formula>F19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I23">
+    <cfRule type="cellIs" dxfId="1" priority="148" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="145" operator="lessThan">
-      <formula>F22</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I23">
-    <cfRule type="cellIs" dxfId="1" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="149" operator="lessThan">
+      <formula>F23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24">
+    <cfRule type="cellIs" dxfId="1" priority="151" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="148" operator="lessThan">
-      <formula>F23</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I24">
-    <cfRule type="cellIs" dxfId="1" priority="150" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="152" operator="lessThan">
+      <formula>F24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I25">
+    <cfRule type="cellIs" dxfId="1" priority="154" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="151" operator="lessThan">
-      <formula>F24</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I25">
-    <cfRule type="cellIs" dxfId="1" priority="153" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="155" operator="lessThan">
+      <formula>F25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I26">
+    <cfRule type="cellIs" dxfId="1" priority="157" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="154" operator="lessThan">
-      <formula>F25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I26">
-    <cfRule type="cellIs" dxfId="1" priority="156" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="158" operator="lessThan">
+      <formula>F26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I27">
+    <cfRule type="cellIs" dxfId="1" priority="160" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="157" operator="lessThan">
-      <formula>F26</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I27">
-    <cfRule type="cellIs" dxfId="1" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="161" operator="lessThan">
+      <formula>F27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I28">
+    <cfRule type="cellIs" dxfId="1" priority="163" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="160" operator="lessThan">
-      <formula>F27</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I29">
-    <cfRule type="cellIs" dxfId="1" priority="162" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="164" operator="lessThan">
+      <formula>F28</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I30">
+    <cfRule type="cellIs" dxfId="1" priority="166" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="163" operator="lessThan">
-      <formula>F29</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I32">
-    <cfRule type="cellIs" dxfId="1" priority="165" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="167" operator="lessThan">
+      <formula>F30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I33">
+    <cfRule type="cellIs" dxfId="1" priority="169" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="166" operator="lessThan">
-      <formula>F32</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I33">
-    <cfRule type="cellIs" dxfId="1" priority="168" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="170" operator="lessThan">
+      <formula>F33</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I34">
+    <cfRule type="cellIs" dxfId="1" priority="172" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="169" operator="lessThan">
-      <formula>F33</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I34">
-    <cfRule type="cellIs" dxfId="1" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="173" operator="lessThan">
+      <formula>F34</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I35">
+    <cfRule type="cellIs" dxfId="1" priority="175" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="172" operator="lessThan">
-      <formula>F34</formula>
+    <cfRule type="cellIs" dxfId="2" priority="176" operator="lessThan">
+      <formula>F35</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="cellIs" dxfId="1" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="121" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="118" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="122" operator="lessThan">
       <formula>F7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="1" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="124" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="121" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="125" operator="lessThan">
       <formula>F8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="cellIs" dxfId="1" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="127" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="124" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="128" operator="lessThan">
       <formula>F9</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J10">
-    <cfRule type="cellIs" dxfId="1" priority="128" operator="greaterThan">
-      <formula>I10</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="J11">
-    <cfRule type="cellIs" dxfId="1" priority="131" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="132" operator="greaterThan">
       <formula>I11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="cellIs" dxfId="1" priority="134" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="135" operator="greaterThan">
       <formula>I12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="cellIs" dxfId="1" priority="137" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="138" operator="greaterThan">
       <formula>I13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14">
-    <cfRule type="cellIs" dxfId="1" priority="140" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="141" operator="greaterThan">
       <formula>I14</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J18">
-    <cfRule type="cellIs" dxfId="1" priority="143" operator="greaterThan">
-      <formula>I18</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J22">
-    <cfRule type="cellIs" dxfId="1" priority="146" operator="greaterThan">
-      <formula>I22</formula>
+  <conditionalFormatting sqref="J15">
+    <cfRule type="cellIs" dxfId="1" priority="144" operator="greaterThan">
+      <formula>I15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J19">
+    <cfRule type="cellIs" dxfId="1" priority="147" operator="greaterThan">
+      <formula>I19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J23">
-    <cfRule type="cellIs" dxfId="1" priority="149" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="150" operator="greaterThan">
       <formula>I23</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24">
-    <cfRule type="cellIs" dxfId="1" priority="152" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="153" operator="greaterThan">
       <formula>I24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J25">
-    <cfRule type="cellIs" dxfId="1" priority="155" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="156" operator="greaterThan">
       <formula>I25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J26">
-    <cfRule type="cellIs" dxfId="1" priority="158" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="159" operator="greaterThan">
       <formula>I26</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J27">
-    <cfRule type="cellIs" dxfId="1" priority="161" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="162" operator="greaterThan">
       <formula>I27</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J29">
-    <cfRule type="cellIs" dxfId="1" priority="164" operator="greaterThan">
-      <formula>I29</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J32">
-    <cfRule type="cellIs" dxfId="1" priority="167" operator="greaterThan">
-      <formula>I32</formula>
+  <conditionalFormatting sqref="J28">
+    <cfRule type="cellIs" dxfId="1" priority="165" operator="greaterThan">
+      <formula>I28</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J30">
+    <cfRule type="cellIs" dxfId="1" priority="168" operator="greaterThan">
+      <formula>I30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J33">
-    <cfRule type="cellIs" dxfId="1" priority="170" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="171" operator="greaterThan">
       <formula>I33</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J34">
-    <cfRule type="cellIs" dxfId="1" priority="173" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="174" operator="greaterThan">
       <formula>I34</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="J35">
+    <cfRule type="cellIs" dxfId="1" priority="177" operator="greaterThan">
+      <formula>I35</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="J7">
-    <cfRule type="cellIs" dxfId="1" priority="119" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="123" operator="greaterThan">
       <formula>I7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="cellIs" dxfId="1" priority="122" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="126" operator="greaterThan">
       <formula>I8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="cellIs" dxfId="1" priority="125" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="129" operator="greaterThan">
       <formula>I9</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3829,37 +3880,37 @@
     <hyperlink ref="M8" r:id="rId3"/>
     <hyperlink ref="E9" r:id="rId4"/>
     <hyperlink ref="M9" r:id="rId5"/>
-    <hyperlink ref="E10" r:id="rId6"/>
-    <hyperlink ref="M10" r:id="rId7"/>
-    <hyperlink ref="E11" r:id="rId8"/>
-    <hyperlink ref="M11" r:id="rId9"/>
-    <hyperlink ref="E12" r:id="rId10"/>
-    <hyperlink ref="M12" r:id="rId11"/>
-    <hyperlink ref="E13" r:id="rId12"/>
-    <hyperlink ref="M13" r:id="rId13"/>
-    <hyperlink ref="E14" r:id="rId14"/>
-    <hyperlink ref="M14" r:id="rId15"/>
-    <hyperlink ref="M18" r:id="rId16"/>
-    <hyperlink ref="E22" r:id="rId17"/>
-    <hyperlink ref="M22" r:id="rId18"/>
-    <hyperlink ref="E23" r:id="rId19"/>
-    <hyperlink ref="M23" r:id="rId20"/>
-    <hyperlink ref="E24" r:id="rId21"/>
-    <hyperlink ref="M24" r:id="rId22"/>
-    <hyperlink ref="E25" r:id="rId23"/>
-    <hyperlink ref="M25" r:id="rId24"/>
-    <hyperlink ref="E26" r:id="rId25"/>
-    <hyperlink ref="M26" r:id="rId26"/>
-    <hyperlink ref="E27" r:id="rId27"/>
-    <hyperlink ref="M27" r:id="rId28"/>
-    <hyperlink ref="E29" r:id="rId29"/>
-    <hyperlink ref="M29" r:id="rId30"/>
-    <hyperlink ref="E32" r:id="rId31"/>
-    <hyperlink ref="M32" r:id="rId32"/>
-    <hyperlink ref="E33" r:id="rId33"/>
-    <hyperlink ref="M33" r:id="rId34"/>
-    <hyperlink ref="E34" r:id="rId35"/>
-    <hyperlink ref="M34" r:id="rId36"/>
+    <hyperlink ref="E11" r:id="rId6"/>
+    <hyperlink ref="M11" r:id="rId7"/>
+    <hyperlink ref="E12" r:id="rId8"/>
+    <hyperlink ref="M12" r:id="rId9"/>
+    <hyperlink ref="E13" r:id="rId10"/>
+    <hyperlink ref="M13" r:id="rId11"/>
+    <hyperlink ref="E14" r:id="rId12"/>
+    <hyperlink ref="M14" r:id="rId13"/>
+    <hyperlink ref="E15" r:id="rId14"/>
+    <hyperlink ref="M15" r:id="rId15"/>
+    <hyperlink ref="M19" r:id="rId16"/>
+    <hyperlink ref="E23" r:id="rId17"/>
+    <hyperlink ref="M23" r:id="rId18"/>
+    <hyperlink ref="E24" r:id="rId19"/>
+    <hyperlink ref="M24" r:id="rId20"/>
+    <hyperlink ref="E25" r:id="rId21"/>
+    <hyperlink ref="M25" r:id="rId22"/>
+    <hyperlink ref="E26" r:id="rId23"/>
+    <hyperlink ref="M26" r:id="rId24"/>
+    <hyperlink ref="E27" r:id="rId25"/>
+    <hyperlink ref="M27" r:id="rId26"/>
+    <hyperlink ref="E28" r:id="rId27"/>
+    <hyperlink ref="M28" r:id="rId28"/>
+    <hyperlink ref="E30" r:id="rId29"/>
+    <hyperlink ref="M30" r:id="rId30"/>
+    <hyperlink ref="E33" r:id="rId31"/>
+    <hyperlink ref="M33" r:id="rId32"/>
+    <hyperlink ref="E34" r:id="rId33"/>
+    <hyperlink ref="M34" r:id="rId34"/>
+    <hyperlink ref="E35" r:id="rId35"/>
+    <hyperlink ref="M35" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId37"/>

</xml_diff>

<commit_message>
Updates bom and kicost for rev3
</commit_message>
<xml_diff>
--- a/board/electrospinner-pcb/electrospinner.xlsx
+++ b/board/electrospinner-pcb/electrospinner.xlsx
@@ -11,8 +11,8 @@
   </sheets>
   <definedNames>
     <definedName name="BoardQty">'electrospinner. '!$H$1</definedName>
-    <definedName name="global_part_data">'electrospinner. '!$A$5:$H$36</definedName>
-    <definedName name="mouser_part_data">'electrospinner. '!$I$5:$M$36</definedName>
+    <definedName name="global_part_data">'electrospinner. '!$A$5:$H$35</definedName>
+    <definedName name="mouser_part_data">'electrospinner. '!$I$5:$M$35</definedName>
     <definedName name="TotalCost">'electrospinner. '!$H$3</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -294,7 +294,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K11" authorId="0">
+    <comment ref="K10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -315,7 +315,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K12" authorId="0">
+    <comment ref="K11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -336,7 +336,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K13" authorId="0">
+    <comment ref="K12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -357,7 +357,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K14" authorId="0">
+    <comment ref="K13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -378,7 +378,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K15" authorId="0">
+    <comment ref="K14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -399,7 +399,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K19" authorId="0">
+    <comment ref="K18" authorId="0">
       <text>
         <r>
           <rPr>
@@ -420,7 +420,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K23" authorId="0">
+    <comment ref="K22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -441,7 +441,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K24" authorId="0">
+    <comment ref="K23" authorId="0">
       <text>
         <r>
           <rPr>
@@ -462,7 +462,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K25" authorId="0">
+    <comment ref="K24" authorId="0">
       <text>
         <r>
           <rPr>
@@ -483,7 +483,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K26" authorId="0">
+    <comment ref="K25" authorId="0">
       <text>
         <r>
           <rPr>
@@ -504,7 +504,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K27" authorId="0">
+    <comment ref="K26" authorId="0">
       <text>
         <r>
           <rPr>
@@ -525,7 +525,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K28" authorId="0">
+    <comment ref="K27" authorId="0">
       <text>
         <r>
           <rPr>
@@ -546,7 +546,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="K30" authorId="0">
+    <comment ref="I29" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This part is listed but is not normally stocked.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K29" authorId="0">
       <text>
         <r>
           <rPr>
@@ -567,7 +580,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K33" authorId="0">
+    <comment ref="K32" authorId="0">
       <text>
         <r>
           <rPr>
@@ -588,7 +601,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K34" authorId="0">
+    <comment ref="K33" authorId="0">
       <text>
         <r>
           <rPr>
@@ -609,7 +622,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K35" authorId="0">
+    <comment ref="K34" authorId="0">
       <text>
         <r>
           <rPr>
@@ -630,7 +643,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G38" authorId="0">
+    <comment ref="G37" authorId="0">
       <text>
         <r>
           <rPr>
@@ -643,7 +656,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J38" authorId="0">
+    <comment ref="J37" authorId="0">
       <text>
         <r>
           <rPr>
@@ -661,7 +674,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="146">
   <si>
     <t>Global Part Info</t>
   </si>
@@ -732,9 +745,6 @@
     <t>AS0805KKX7R9BB104</t>
   </si>
   <si>
-    <t>C11</t>
-  </si>
-  <si>
     <t>C2</t>
   </si>
   <si>
@@ -768,7 +778,7 @@
     <t>CGA4J1X8L1C335K125AC</t>
   </si>
   <si>
-    <t>C5,C7-C10</t>
+    <t>C5,C7-C11</t>
   </si>
   <si>
     <t>Capacitor_SMD:C_0603_1608Metric</t>
@@ -1011,7 +1021,7 @@
     <t>Prj date:</t>
   </si>
   <si>
-    <t>Mon 08 Apr 2019 04:11:23 PM EDT</t>
+    <t>Tue 09 Apr 2019 01:19:35 PM EDT</t>
   </si>
   <si>
     <t>Board Qty:</t>
@@ -1026,7 +1036,7 @@
     <t>$ date:</t>
   </si>
   <si>
-    <t>2019-04-08 16:11:31</t>
+    <t>2019-04-09 13:20:00</t>
   </si>
   <si>
     <t>Mouser</t>
@@ -1086,7 +1096,10 @@
     <t>660-SG73G2ATTD1001D</t>
   </si>
   <si>
-    <t>836-1200</t>
+    <t>502-1200</t>
+  </si>
+  <si>
+    <t>NonStk</t>
   </si>
   <si>
     <t>895-FT230XS-R</t>
@@ -1110,7 +1123,7 @@
     <numFmt numFmtId="164" formatCode="$#,##0.00"/>
     <numFmt numFmtId="164" formatCode="$#,##0.00"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1187,6 +1200,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF909090"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1224,7 +1244,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1261,6 +1281,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1591,7 +1614,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M68"/>
+  <dimension ref="A1:M66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="8" ySplit="6" topLeftCell="I7" activePane="bottomRight" state="frozen"/>
@@ -1619,13 +1642,13 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="G1" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H1" s="4">
         <v>100</v>
@@ -1633,13 +1656,13 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>114</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H2" s="5">
         <f>TotalCost/BoardQty</f>
@@ -1648,33 +1671,33 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>116</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H3" s="6">
-        <f>SUM(H7:H36)</f>
+        <f>SUM(H7:H35)</f>
         <v>0</v>
       </c>
       <c r="L3" s="6">
-        <f>SUM(L7:L36)</f>
+        <f>SUM(L7:L35)</f>
         <v>0</v>
       </c>
       <c r="M3" s="7">
-        <f>(ROWS(L7:L36)-COUNTBLANK(L7:L36))&amp;" of "&amp;ROWS(L7:L36)&amp;" parts found"</f>
+        <f>(ROWS(L7:L35)-COUNTBLANK(L7:L35))&amp;" of "&amp;ROWS(L7:L35)&amp;" parts found"</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1689,7 +1712,7 @@
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
@@ -1722,10 +1745,10 @@
         <v>8</v>
       </c>
       <c r="I6" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="J6" s="10" t="s">
         <v>123</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>124</v>
       </c>
       <c r="K6" s="10" t="s">
         <v>7</v>
@@ -1734,7 +1757,7 @@
         <v>8</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1777,7 +1800,7 @@
         <v>0</v>
       </c>
       <c r="M7" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -1817,7 +1840,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -1860,7 +1883,7 @@
         <v>0</v>
       </c>
       <c r="M9" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -1868,7 +1891,13 @@
         <v>23</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>19</v>
+        <v>24</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="F10" s="11">
         <f>BoardQty*1</f>
@@ -1882,19 +1911,36 @@
         <f>iferror(F10*G10,"")</f>
         <v>0</v>
       </c>
+      <c r="I10" s="11">
+        <v>35924</v>
+      </c>
+      <c r="K10" s="12">
+        <f>iferror(lookup(if(J10="",F10,J10),{0,1,10,50,100,1000,10000},{0.0,1.06,0.75,0.75,0.473,0.388,0.24700000000000003}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="12">
+        <f>iferror(if(J10="",F10,J10)*K10,"")</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="13" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>20</v>
+        <v>28</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>29</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F11" s="11">
         <f>BoardQty*1</f>
@@ -1909,10 +1955,10 @@
         <v>0</v>
       </c>
       <c r="I11" s="11">
-        <v>35924</v>
+        <v>3769</v>
       </c>
       <c r="K11" s="12">
-        <f>iferror(lookup(if(J11="",F11,J11),{0,1,10,50,100,1000,10000},{0.0,1.06,0.75,0.75,0.473,0.388,0.24700000000000003}),"")</f>
+        <f>iferror(lookup(if(J11="",F11,J11),{0,1,10,50,100,1000,10000},{0.0,0.6000000000000001,0.483,0.483,0.276,0.174,0.143}),"")</f>
         <v>0</v>
       </c>
       <c r="L11" s="12">
@@ -1925,19 +1971,16 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F12" s="11">
         <f>BoardQty*1</f>
@@ -1952,10 +1995,10 @@
         <v>0</v>
       </c>
       <c r="I12" s="11">
-        <v>3769</v>
+        <v>2644</v>
       </c>
       <c r="K12" s="12">
-        <f>iferror(lookup(if(J12="",F12,J12),{0,1,10,50,100,1000,10000},{0.0,0.6000000000000001,0.483,0.483,0.276,0.174,0.143}),"")</f>
+        <f>iferror(lookup(if(J12="",F12,J12),{0,1,10,50,100,1000,10000},{0.0,0.59,0.344,0.344,0.233,0.194,0.11899999999999998}),"")</f>
         <v>0</v>
       </c>
       <c r="L12" s="12">
@@ -1968,19 +2011,22 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>20</v>
+        <v>35</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>36</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F13" s="11">
-        <f>BoardQty*1</f>
+        <f>BoardQty*6</f>
         <v>0</v>
       </c>
       <c r="G13" s="12">
@@ -1992,10 +2038,10 @@
         <v>0</v>
       </c>
       <c r="I13" s="11">
-        <v>2644</v>
+        <v>378604</v>
       </c>
       <c r="K13" s="12">
-        <f>iferror(lookup(if(J13="",F13,J13),{0,1,10,50,100,1000,10000},{0.0,0.59,0.344,0.344,0.233,0.194,0.11899999999999998}),"")</f>
+        <f>iferror(lookup(if(J13="",F13,J13),{0,1,10,50,100,1000,10000},{0.0,0.24,0.113,0.113,0.076,0.062,0.042}),"")</f>
         <v>0</v>
       </c>
       <c r="L13" s="12">
@@ -2008,22 +2054,19 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="11" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F14" s="11">
-        <f>BoardQty*5</f>
+        <f>BoardQty*1</f>
         <v>0</v>
       </c>
       <c r="G14" s="12">
@@ -2035,10 +2078,10 @@
         <v>0</v>
       </c>
       <c r="I14" s="11">
-        <v>378604</v>
+        <v>6838</v>
       </c>
       <c r="K14" s="12">
-        <f>iferror(lookup(if(J14="",F14,J14),{0,1,10,50,100,1000,10000},{0.0,0.24,0.113,0.113,0.076,0.062,0.042}),"")</f>
+        <f>iferror(lookup(if(J14="",F14,J14),{0,1,10,50,100,1000,10000},{0.0,0.38,0.264,0.264,0.15000000000000002,0.092,0.069}),"")</f>
         <v>0</v>
       </c>
       <c r="L14" s="12">
@@ -2051,16 +2094,13 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F15" s="11">
         <f>BoardQty*1</f>
@@ -2074,30 +2114,16 @@
         <f>iferror(F15*G15,"")</f>
         <v>0</v>
       </c>
-      <c r="I15" s="11">
-        <v>6838</v>
-      </c>
-      <c r="K15" s="12">
-        <f>iferror(lookup(if(J15="",F15,J15),{0,1,10,50,100,1000,10000},{0.0,0.38,0.264,0.264,0.15000000000000002,0.092,0.069}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="L15" s="12">
-        <f>iferror(if(J15="",F15,J15)*K15,"")</f>
-        <v>0</v>
-      </c>
-      <c r="M15" s="13" t="s">
-        <v>133</v>
-      </c>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="11" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B16" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>43</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>44</v>
       </c>
       <c r="F16" s="11">
         <f>BoardQty*1</f>
@@ -2114,13 +2140,13 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F17" s="11">
         <f>BoardQty*1</f>
@@ -2137,13 +2163,16 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="F18" s="11">
         <f>BoardQty*1</f>
@@ -2157,19 +2186,30 @@
         <f>iferror(F18*G18,"")</f>
         <v>0</v>
       </c>
+      <c r="I18" s="11">
+        <v>5135</v>
+      </c>
+      <c r="K18" s="12">
+        <f>iferror(lookup(if(J18="",F18,J18),{0,1,10,50,100,1000,10000},{0.0,0.73,0.637,0.637,0.45400000000000007,0.269,0.237}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="L18" s="12">
+        <f>iferror(if(J18="",F18,J18)*K18,"")</f>
+        <v>0</v>
+      </c>
+      <c r="M18" s="13" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="11" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F19" s="11">
         <f>BoardQty*1</f>
@@ -2183,30 +2223,13 @@
         <f>iferror(F19*G19,"")</f>
         <v>0</v>
       </c>
-      <c r="I19" s="11">
-        <v>5135</v>
-      </c>
-      <c r="K19" s="12">
-        <f>iferror(lookup(if(J19="",F19,J19),{0,1,10,50,100,1000,10000},{0.0,0.73,0.637,0.637,0.45400000000000007,0.269,0.237}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="L19" s="12">
-        <f>iferror(if(J19="",F19,J19)*K19,"")</f>
-        <v>0</v>
-      </c>
-      <c r="M19" s="13" t="s">
-        <v>134</v>
-      </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="11" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F20" s="11">
         <f>BoardQty*1</f>
@@ -2223,10 +2246,16 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>61</v>
       </c>
       <c r="F21" s="11">
         <f>BoardQty*1</f>
@@ -2243,16 +2272,19 @@
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="11" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>60</v>
+        <v>63</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>64</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F22" s="11">
         <f>BoardQty*1</f>
@@ -2266,22 +2298,36 @@
         <f>iferror(F22*G22,"")</f>
         <v>0</v>
       </c>
+      <c r="I22" s="11">
+        <v>113570</v>
+      </c>
+      <c r="K22" s="12">
+        <f>iferror(lookup(if(J22="",F22,J22),{0,1,10,50,100,1000,10000},{0.0,0.1,0.031,0.031,0.017,0.009999999999999998,0.007}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="L22" s="12">
+        <f>iferror(if(J22="",F22,J22)*K22,"")</f>
+        <v>0</v>
+      </c>
+      <c r="M22" s="13" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="11" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="F23" s="11">
         <f>BoardQty*1</f>
@@ -2296,10 +2342,10 @@
         <v>0</v>
       </c>
       <c r="I23" s="11">
-        <v>113570</v>
+        <v>14531</v>
       </c>
       <c r="K23" s="12">
-        <f>iferror(lookup(if(J23="",F23,J23),{0,1,10,50,100,1000,10000},{0.0,0.1,0.031,0.031,0.017,0.009999999999999998,0.007}),"")</f>
+        <f>iferror(lookup(if(J23="",F23,J23),{0,1,10,50,100,1000,10000},{0.0,0.23,0.23,0.17900000000000002,0.154,0.115,0.085}),"")</f>
         <v>0</v>
       </c>
       <c r="L23" s="12">
@@ -2312,19 +2358,16 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="11" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B24" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>71</v>
-      </c>
       <c r="E24" s="11" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F24" s="11">
         <f>BoardQty*1</f>
@@ -2339,10 +2382,10 @@
         <v>0</v>
       </c>
       <c r="I24" s="11">
-        <v>14531</v>
+        <v>9459</v>
       </c>
       <c r="K24" s="12">
-        <f>iferror(lookup(if(J24="",F24,J24),{0,1,10,50,100,1000,10000},{0.0,0.23,0.23,0.17900000000000002,0.154,0.115,0.085}),"")</f>
+        <f>iferror(lookup(if(J24="",F24,J24),{0,1,10,50,100,1000,10000},{0.0,0.14,0.077,0.064,0.043,0.019999999999999997,0.019999999999999997}),"")</f>
         <v>0</v>
       </c>
       <c r="L24" s="12">
@@ -2355,16 +2398,16 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="11" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F25" s="11">
         <f>BoardQty*1</f>
@@ -2379,10 +2422,10 @@
         <v>0</v>
       </c>
       <c r="I25" s="11">
-        <v>9459</v>
+        <v>57541</v>
       </c>
       <c r="K25" s="12">
-        <f>iferror(lookup(if(J25="",F25,J25),{0,1,10,50,100,1000,10000},{0.0,0.14,0.077,0.064,0.043,0.019999999999999997,0.019999999999999997}),"")</f>
+        <f>iferror(lookup(if(J25="",F25,J25),{0,1,10,50,100,1000,10000},{0.0,0.14,0.065,0.065,0.035,0.012,0.006}),"")</f>
         <v>0</v>
       </c>
       <c r="L25" s="12">
@@ -2395,19 +2438,19 @@
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="11" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F26" s="11">
-        <f>BoardQty*1</f>
+        <f>BoardQty*2</f>
         <v>0</v>
       </c>
       <c r="G26" s="12">
@@ -2419,10 +2462,10 @@
         <v>0</v>
       </c>
       <c r="I26" s="11">
-        <v>57541</v>
+        <v>9584</v>
       </c>
       <c r="K26" s="12">
-        <f>iferror(lookup(if(J26="",F26,J26),{0,1,10,50,100,1000,10000},{0.0,0.14,0.065,0.065,0.035,0.012,0.006}),"")</f>
+        <f>iferror(lookup(if(J26="",F26,J26),{0,1,10,50,100,1000,10000},{0.0,0.14,0.077,0.064,0.043,0.019999999999999997,0.019999999999999997}),"")</f>
         <v>0</v>
       </c>
       <c r="L26" s="12">
@@ -2435,19 +2478,19 @@
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="11" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F27" s="11">
-        <f>BoardQty*2</f>
+        <f>BoardQty*1</f>
         <v>0</v>
       </c>
       <c r="G27" s="12">
@@ -2459,10 +2502,10 @@
         <v>0</v>
       </c>
       <c r="I27" s="11">
-        <v>9584</v>
+        <v>5375</v>
       </c>
       <c r="K27" s="12">
-        <f>iferror(lookup(if(J27="",F27,J27),{0,1,10,50,100,1000,10000},{0.0,0.14,0.077,0.064,0.043,0.019999999999999997,0.019999999999999997}),"")</f>
+        <f>iferror(lookup(if(J27="",F27,J27),{0,1,10,50,100,1000,10000},{0.0,0.23,0.23,0.17900000000000002,0.154,0.115,0.085}),"")</f>
         <v>0</v>
       </c>
       <c r="L27" s="12">
@@ -2475,16 +2518,13 @@
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="11" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F28" s="11">
         <f>BoardQty*1</f>
@@ -2498,30 +2538,19 @@
         <f>iferror(F28*G28,"")</f>
         <v>0</v>
       </c>
-      <c r="I28" s="11">
-        <v>5375</v>
-      </c>
-      <c r="K28" s="12">
-        <f>iferror(lookup(if(J28="",F28,J28),{0,1,10,50,100,1000,10000},{0.0,0.23,0.23,0.17900000000000002,0.154,0.115,0.085}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="L28" s="12">
-        <f>iferror(if(J28="",F28,J28)*K28,"")</f>
-        <v>0</v>
-      </c>
-      <c r="M28" s="13" t="s">
-        <v>140</v>
-      </c>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="11" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>87</v>
+        <v>88</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>89</v>
       </c>
       <c r="F29" s="11">
         <f>BoardQty*1</f>
@@ -2535,19 +2564,30 @@
         <f>iferror(F29*G29,"")</f>
         <v>0</v>
       </c>
+      <c r="I29" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="K29" s="12">
+        <f>iferror(lookup(if(J29="",F29,J29),{0,1,10,50,100,1000,10000},{0.0,0.35,0.334,0.242,0.233,0.166,0.143}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="L29" s="12">
+        <f>iferror(if(J29="",F29,J29)*K29,"")</f>
+        <v>0</v>
+      </c>
+      <c r="M29" s="13" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="11" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>90</v>
+        <v>91</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>92</v>
       </c>
       <c r="F30" s="11">
         <f>BoardQty*1</f>
@@ -2561,30 +2601,13 @@
         <f>iferror(F30*G30,"")</f>
         <v>0</v>
       </c>
-      <c r="I30" s="11">
-        <v>26048</v>
-      </c>
-      <c r="K30" s="12">
-        <f>iferror(lookup(if(J30="",F30,J30),{0,1,10,50,100,1000,10000},{0.0,0.35,0.334,0.242,0.233,0.166,0.143}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="L30" s="12">
-        <f>iferror(if(J30="",F30,J30)*K30,"")</f>
-        <v>0</v>
-      </c>
-      <c r="M30" s="13" t="s">
-        <v>141</v>
-      </c>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="11" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F31" s="11">
         <f>BoardQty*1</f>
@@ -2601,10 +2624,16 @@
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>98</v>
       </c>
       <c r="F32" s="11">
         <f>BoardQty*1</f>
@@ -2618,19 +2647,33 @@
         <f>iferror(F32*G32,"")</f>
         <v>0</v>
       </c>
+      <c r="I32" s="11">
+        <v>105821</v>
+      </c>
+      <c r="K32" s="12">
+        <f>iferror(lookup(if(J32="",F32,J32),{0,1,10,50,100,1000,10000},{0.0,2.04,2.04,1.97,1.9000000000000001,1.46,1.4}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="L32" s="12">
+        <f>iferror(if(J32="",F32,J32)*K32,"")</f>
+        <v>0</v>
+      </c>
+      <c r="M32" s="13" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="11" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F33" s="11">
         <f>BoardQty*1</f>
@@ -2645,10 +2688,10 @@
         <v>0</v>
       </c>
       <c r="I33" s="11">
-        <v>106176</v>
+        <v>26496</v>
       </c>
       <c r="K33" s="12">
-        <f>iferror(lookup(if(J33="",F33,J33),{0,1,10,50,100,1000,10000},{0.0,2.04,2.04,1.97,1.9000000000000001,1.46,1.4}),"")</f>
+        <f>iferror(lookup(if(J33="",F33,J33),{0,1,10,50,100,1000,10000},{0.0,2.15,1.83,1.83,1.46,1.06,0.949}),"")</f>
         <v>0</v>
       </c>
       <c r="L33" s="12">
@@ -2656,21 +2699,21 @@
         <v>0</v>
       </c>
       <c r="M33" s="13" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="11" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F34" s="11">
         <f>BoardQty*1</f>
@@ -2685,10 +2728,10 @@
         <v>0</v>
       </c>
       <c r="I34" s="11">
-        <v>26496</v>
+        <v>1771</v>
       </c>
       <c r="K34" s="12">
-        <f>iferror(lookup(if(J34="",F34,J34),{0,1,10,50,100,1000,10000},{0.0,2.15,1.83,1.83,1.46,1.06,0.949}),"")</f>
+        <f>iferror(lookup(if(J34="",F34,J34),{0,1,10,50,100,1000,10000},{0.0,2.46,2.09,2.09,1.68,1.22,1.09}),"")</f>
         <v>0</v>
       </c>
       <c r="L34" s="12">
@@ -2696,21 +2739,18 @@
         <v>0</v>
       </c>
       <c r="M34" s="13" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="11" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F35" s="11">
         <f>BoardQty*1</f>
@@ -2724,481 +2764,430 @@
         <f>iferror(F35*G35,"")</f>
         <v>0</v>
       </c>
-      <c r="I35" s="11">
-        <v>1771</v>
-      </c>
-      <c r="K35" s="12">
-        <f>iferror(lookup(if(J35="",F35,J35),{0,1,10,50,100,1000,10000},{0.0,2.46,2.09,2.09,1.68,1.22,1.09}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="L35" s="12">
-        <f>iferror(if(J35="",F35,J35)*K35,"")</f>
-        <v>0</v>
-      </c>
-      <c r="M35" s="13" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13">
-      <c r="A36" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="C36" s="11" t="s">
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G37" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F36" s="11">
-        <f>BoardQty*1</f>
-        <v>0</v>
-      </c>
-      <c r="G36" s="12">
-        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0</v>
-      </c>
-      <c r="H36" s="12">
-        <f>iferror(F36*G36,"")</f>
+      <c r="H37" s="6">
+        <f>SUM(INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+3)))</f>
+        <v>0</v>
+      </c>
+      <c r="J37" s="7">
+        <f>IFERROR(IF(OR(J7:J35),COUNTIFS(J7:J35,"&gt;0",L7:L35,"&lt;&gt;")&amp;" of "&amp;(ROWS(L7:L35)-COUNTBLANK(L7:L35))&amp;" parts purchased",""),"")</f>
+        <v>0</v>
+      </c>
+      <c r="L37" s="6">
+        <f>SUMIF(J7:J35,"&gt;0",L7:L35)</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:13">
-      <c r="A38" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="H38" s="6">
-        <f>SUM(INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+3)))</f>
-        <v>0</v>
-      </c>
-      <c r="J38" s="7">
-        <f>IFERROR(IF(OR(J7:J36),COUNTIFS(J7:J36,"&gt;0",L7:L36,"&lt;&gt;")&amp;" of "&amp;(ROWS(L7:L36)-COUNTBLANK(L7:L36))&amp;" parts purchased",""),"")</f>
-        <v>0</v>
-      </c>
-      <c r="L38" s="6">
-        <f>SUMIF(J7:J36,"&gt;0",L7:L36)</f>
+      <c r="J38">
+        <f t="array" ref="J38">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <f t="array" ref="K38">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
+        <v>0</v>
+      </c>
+      <c r="L38">
+        <f t="array" ref="L38">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:13">
       <c r="J39">
-        <f t="array" ref="J39">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <f t="array" ref="J39">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K39">
-        <f t="array" ref="K39">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K39">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L39">
-        <f t="array" ref="L39">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <f t="array" ref="L39">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:13">
       <c r="J40">
-        <f t="array" ref="J40">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <f t="array" ref="J40">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K40">
-        <f t="array" ref="K40">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K40">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L40">
-        <f t="array" ref="L40">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <f t="array" ref="L40">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:13">
       <c r="J41">
-        <f t="array" ref="J41">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <f t="array" ref="J41">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K41">
-        <f t="array" ref="K41">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K41">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L41">
-        <f t="array" ref="L41">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <f t="array" ref="L41">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:13">
       <c r="J42">
-        <f t="array" ref="J42">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <f t="array" ref="J42">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K42">
-        <f t="array" ref="K42">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K42">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L42">
-        <f t="array" ref="L42">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <f t="array" ref="L42">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:13">
       <c r="J43">
-        <f t="array" ref="J43">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <f t="array" ref="J43">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K43">
-        <f t="array" ref="K43">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K43">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L43">
-        <f t="array" ref="L43">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <f t="array" ref="L43">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:13">
       <c r="J44">
-        <f t="array" ref="J44">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <f t="array" ref="J44">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K44">
-        <f t="array" ref="K44">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K44">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L44">
-        <f t="array" ref="L44">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <f t="array" ref="L44">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:13">
       <c r="J45">
-        <f t="array" ref="J45">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <f t="array" ref="J45">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K45">
-        <f t="array" ref="K45">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K45">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L45">
-        <f t="array" ref="L45">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <f t="array" ref="L45">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:13">
       <c r="J46">
-        <f t="array" ref="J46">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <f t="array" ref="J46">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K46">
-        <f t="array" ref="K46">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K46">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L46">
-        <f t="array" ref="L46">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <f t="array" ref="L46">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:13">
       <c r="J47">
-        <f t="array" ref="J47">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <f t="array" ref="J47">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K47">
-        <f t="array" ref="K47">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K47">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L47">
-        <f t="array" ref="L47">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <f t="array" ref="L47">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:13">
       <c r="J48">
-        <f t="array" ref="J48">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <f t="array" ref="J48">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K48">
-        <f t="array" ref="K48">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K48">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L48">
-        <f t="array" ref="L48">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <f t="array" ref="L48">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="10:12">
       <c r="J49">
-        <f t="array" ref="J49">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <f t="array" ref="J49">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K49">
-        <f t="array" ref="K49">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K49">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L49">
-        <f t="array" ref="L49">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <f t="array" ref="L49">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="10:12">
       <c r="J50">
-        <f t="array" ref="J50">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <f t="array" ref="J50">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K50">
-        <f t="array" ref="K50">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K50">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L50">
-        <f t="array" ref="L50">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <f t="array" ref="L50">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="10:12">
       <c r="J51">
-        <f t="array" ref="J51">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <f t="array" ref="J51">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K51">
-        <f t="array" ref="K51">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K51">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L51">
-        <f t="array" ref="L51">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <f t="array" ref="L51">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="10:12">
       <c r="J52">
-        <f t="array" ref="J52">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <f t="array" ref="J52">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K52">
-        <f t="array" ref="K52">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K52">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L52">
-        <f t="array" ref="L52">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <f t="array" ref="L52">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="10:12">
       <c r="J53">
-        <f t="array" ref="J53">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <f t="array" ref="J53">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K53">
-        <f t="array" ref="K53">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K53">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L53">
-        <f t="array" ref="L53">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <f t="array" ref="L53">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="10:12">
       <c r="J54">
-        <f t="array" ref="J54">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <f t="array" ref="J54">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K54">
-        <f t="array" ref="K54">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K54">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L54">
-        <f t="array" ref="L54">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <f t="array" ref="L54">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="10:12">
       <c r="J55">
-        <f t="array" ref="J55">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <f t="array" ref="J55">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K55">
-        <f t="array" ref="K55">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K55">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L55">
-        <f t="array" ref="L55">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <f t="array" ref="L55">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="10:12">
       <c r="J56">
-        <f t="array" ref="J56">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <f t="array" ref="J56">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K56">
-        <f t="array" ref="K56">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K56">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L56">
-        <f t="array" ref="L56">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <f t="array" ref="L56">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="10:12">
       <c r="J57">
-        <f t="array" ref="J57">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <f t="array" ref="J57">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K57">
-        <f t="array" ref="K57">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K57">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L57">
-        <f t="array" ref="L57">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <f t="array" ref="L57">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="10:12">
       <c r="J58">
-        <f t="array" ref="J58">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <f t="array" ref="J58">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K58">
-        <f t="array" ref="K58">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K58">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L58">
-        <f t="array" ref="L58">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <f t="array" ref="L58">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="10:12">
       <c r="J59">
-        <f t="array" ref="J59">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <f t="array" ref="J59">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K59">
-        <f t="array" ref="K59">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K59">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L59">
-        <f t="array" ref="L59">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <f t="array" ref="L59">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="10:12">
       <c r="J60">
-        <f t="array" ref="J60">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <f t="array" ref="J60">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K60">
-        <f t="array" ref="K60">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K60">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L60">
-        <f t="array" ref="L60">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <f t="array" ref="L60">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="10:12">
       <c r="J61">
-        <f t="array" ref="J61">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <f t="array" ref="J61">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K61">
-        <f t="array" ref="K61">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K61">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L61">
-        <f t="array" ref="L61">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <f t="array" ref="L61">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="10:12">
       <c r="J62">
-        <f t="array" ref="J62">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <f t="array" ref="J62">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K62">
-        <f t="array" ref="K62">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K62">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L62">
-        <f t="array" ref="L62">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <f t="array" ref="L62">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="10:12">
       <c r="J63">
-        <f t="array" ref="J63">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <f t="array" ref="J63">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K63">
-        <f t="array" ref="K63">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K63">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L63">
-        <f t="array" ref="L63">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <f t="array" ref="L63">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="10:12">
       <c r="J64">
-        <f t="array" ref="J64">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <f t="array" ref="J64">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K64">
-        <f t="array" ref="K64">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K64">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L64">
-        <f t="array" ref="L64">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <f t="array" ref="L64">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="10:12">
       <c r="J65">
-        <f t="array" ref="J65">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <f t="array" ref="J65">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K65">
-        <f t="array" ref="K65">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K65">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L65">
-        <f t="array" ref="L65">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <f t="array" ref="L65">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="10:12">
       <c r="J66">
-        <f t="array" ref="J66">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
+        <f t="array" ref="J66">IFERROR(CONCATENATE((INDEX($M$7:$M$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="K66">
-        <f t="array" ref="K66">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
+        <f t="array" ref="K66">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1)),"##0"),"|"),"")</f>
         <v>0</v>
       </c>
       <c r="L66">
-        <f t="array" ref="L66">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="10:12">
-      <c r="J67">
-        <f t="array" ref="J67">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
-        <v>0</v>
-      </c>
-      <c r="K67">
-        <f t="array" ref="K67">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
-        <v>0</v>
-      </c>
-      <c r="L67">
-        <f t="array" ref="L67">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="10:12">
-      <c r="J68">
-        <f t="array" ref="J68">IFERROR(CONCATENATE((INDEX($M$7:$M$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),"|"),"")</f>
-        <v>0</v>
-      </c>
-      <c r="K68">
-        <f t="array" ref="K68">IFERROR(CONCATENATE(TEXT(INDEX($J$7:$J$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1)),"##0"),"|"),"")</f>
-        <v>0</v>
-      </c>
-      <c r="L68">
-        <f t="array" ref="L68">IFERROR(CONCATENATE((INDEX($A$7:$A$36,SMALL(IF($M$7:$M$36&lt;&gt;"",IF($J$7:$J$36&lt;&gt;"",ROW($J$7:$J$36)-MIN(ROW($J$7:$J$36))+1,""),""),ROW()-ROW(A$39)+1))),),"")</f>
+        <f t="array" ref="L66">IFERROR(CONCATENATE((INDEX($A$7:$A$35,SMALL(IF($M$7:$M$35&lt;&gt;"",IF($J$7:$J$35&lt;&gt;"",ROW($J$7:$J$35)-MIN(ROW($J$7:$J$35))+1,""),""),ROW()-ROW(A$38)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
@@ -3571,20 +3560,6 @@
       <formula>SUM(IF(ISNUMBER(INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2))),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+1)),0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F36">
-    <cfRule type="expression" dxfId="0" priority="117">
-      <formula>AND(ISBLANK(E36),ISBLANK(INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+4))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="118">
-      <formula>IF(SUM(INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+0)))=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="119" operator="greaterThan">
-      <formula>SUM(INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+0)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="120" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2))),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+1)),0))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F7">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND(ISBLANK(E7),ISBLANK(INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+4))))</formula>
@@ -3627,250 +3602,250 @@
       <formula>SUM(IF(ISNUMBER(INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2))),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+1)),0))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="I10">
+    <cfRule type="cellIs" dxfId="1" priority="126" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="127" operator="lessThan">
+      <formula>F10</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="cellIs" dxfId="1" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="129" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="131" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="130" operator="lessThan">
       <formula>F11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="cellIs" dxfId="1" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="132" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="134" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="133" operator="lessThan">
       <formula>F12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13">
-    <cfRule type="cellIs" dxfId="1" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="135" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="137" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="136" operator="lessThan">
       <formula>F13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="1" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="138" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="140" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="139" operator="lessThan">
       <formula>F14</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I15">
-    <cfRule type="cellIs" dxfId="1" priority="142" operator="equal">
+  <conditionalFormatting sqref="I18">
+    <cfRule type="cellIs" dxfId="1" priority="141" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="143" operator="lessThan">
-      <formula>F15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I19">
-    <cfRule type="cellIs" dxfId="1" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="142" operator="lessThan">
+      <formula>F18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I22">
+    <cfRule type="cellIs" dxfId="1" priority="144" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="146" operator="lessThan">
-      <formula>F19</formula>
+    <cfRule type="cellIs" dxfId="2" priority="145" operator="lessThan">
+      <formula>F22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23">
-    <cfRule type="cellIs" dxfId="1" priority="148" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="147" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="149" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="148" operator="lessThan">
       <formula>F23</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24">
-    <cfRule type="cellIs" dxfId="1" priority="151" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="150" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="152" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="151" operator="lessThan">
       <formula>F24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I25">
-    <cfRule type="cellIs" dxfId="1" priority="154" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="153" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="155" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="154" operator="lessThan">
       <formula>F25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26">
-    <cfRule type="cellIs" dxfId="1" priority="157" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="156" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="158" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="157" operator="lessThan">
       <formula>F26</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27">
-    <cfRule type="cellIs" dxfId="1" priority="160" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="159" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="161" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="160" operator="lessThan">
       <formula>F27</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I28">
-    <cfRule type="cellIs" dxfId="1" priority="163" operator="equal">
+  <conditionalFormatting sqref="I29">
+    <cfRule type="cellIs" dxfId="1" priority="162" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="164" operator="lessThan">
-      <formula>F28</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I30">
-    <cfRule type="cellIs" dxfId="1" priority="166" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="163" operator="lessThan">
+      <formula>F29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I32">
+    <cfRule type="cellIs" dxfId="1" priority="165" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="167" operator="lessThan">
-      <formula>F30</formula>
+    <cfRule type="cellIs" dxfId="2" priority="166" operator="lessThan">
+      <formula>F32</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33">
-    <cfRule type="cellIs" dxfId="1" priority="169" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="168" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="170" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="169" operator="lessThan">
       <formula>F33</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I34">
-    <cfRule type="cellIs" dxfId="1" priority="172" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="171" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="173" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="172" operator="lessThan">
       <formula>F34</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I35">
-    <cfRule type="cellIs" dxfId="1" priority="175" operator="equal">
+  <conditionalFormatting sqref="I7">
+    <cfRule type="cellIs" dxfId="1" priority="117" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="176" operator="lessThan">
-      <formula>F35</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I7">
-    <cfRule type="cellIs" dxfId="1" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="118" operator="lessThan">
+      <formula>F7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8">
+    <cfRule type="cellIs" dxfId="1" priority="120" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="122" operator="lessThan">
-      <formula>F7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="1" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="121" operator="lessThan">
+      <formula>F8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9">
+    <cfRule type="cellIs" dxfId="1" priority="123" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="125" operator="lessThan">
-      <formula>F8</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I9">
-    <cfRule type="cellIs" dxfId="1" priority="127" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="128" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="124" operator="lessThan">
       <formula>F9</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="J10">
+    <cfRule type="cellIs" dxfId="1" priority="128" operator="greaterThan">
+      <formula>I10</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="J11">
-    <cfRule type="cellIs" dxfId="1" priority="132" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="131" operator="greaterThan">
       <formula>I11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12">
-    <cfRule type="cellIs" dxfId="1" priority="135" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="134" operator="greaterThan">
       <formula>I12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="cellIs" dxfId="1" priority="138" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="137" operator="greaterThan">
       <formula>I13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14">
-    <cfRule type="cellIs" dxfId="1" priority="141" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="140" operator="greaterThan">
       <formula>I14</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J15">
-    <cfRule type="cellIs" dxfId="1" priority="144" operator="greaterThan">
-      <formula>I15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J19">
-    <cfRule type="cellIs" dxfId="1" priority="147" operator="greaterThan">
-      <formula>I19</formula>
+  <conditionalFormatting sqref="J18">
+    <cfRule type="cellIs" dxfId="1" priority="143" operator="greaterThan">
+      <formula>I18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J22">
+    <cfRule type="cellIs" dxfId="1" priority="146" operator="greaterThan">
+      <formula>I22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J23">
-    <cfRule type="cellIs" dxfId="1" priority="150" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="149" operator="greaterThan">
       <formula>I23</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24">
-    <cfRule type="cellIs" dxfId="1" priority="153" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="152" operator="greaterThan">
       <formula>I24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J25">
-    <cfRule type="cellIs" dxfId="1" priority="156" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="155" operator="greaterThan">
       <formula>I25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J26">
-    <cfRule type="cellIs" dxfId="1" priority="159" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="158" operator="greaterThan">
       <formula>I26</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J27">
-    <cfRule type="cellIs" dxfId="1" priority="162" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="161" operator="greaterThan">
       <formula>I27</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J28">
-    <cfRule type="cellIs" dxfId="1" priority="165" operator="greaterThan">
-      <formula>I28</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J30">
-    <cfRule type="cellIs" dxfId="1" priority="168" operator="greaterThan">
-      <formula>I30</formula>
+  <conditionalFormatting sqref="J29">
+    <cfRule type="cellIs" dxfId="1" priority="164" operator="greaterThan">
+      <formula>I29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J32">
+    <cfRule type="cellIs" dxfId="1" priority="167" operator="greaterThan">
+      <formula>I32</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J33">
-    <cfRule type="cellIs" dxfId="1" priority="171" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="170" operator="greaterThan">
       <formula>I33</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J34">
-    <cfRule type="cellIs" dxfId="1" priority="174" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="173" operator="greaterThan">
       <formula>I34</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J35">
-    <cfRule type="cellIs" dxfId="1" priority="177" operator="greaterThan">
-      <formula>I35</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="J7">
-    <cfRule type="cellIs" dxfId="1" priority="123" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="119" operator="greaterThan">
       <formula>I7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="cellIs" dxfId="1" priority="126" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="122" operator="greaterThan">
       <formula>I8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="cellIs" dxfId="1" priority="129" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="125" operator="greaterThan">
       <formula>I9</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3880,37 +3855,37 @@
     <hyperlink ref="M8" r:id="rId3"/>
     <hyperlink ref="E9" r:id="rId4"/>
     <hyperlink ref="M9" r:id="rId5"/>
-    <hyperlink ref="E11" r:id="rId6"/>
-    <hyperlink ref="M11" r:id="rId7"/>
-    <hyperlink ref="E12" r:id="rId8"/>
-    <hyperlink ref="M12" r:id="rId9"/>
-    <hyperlink ref="E13" r:id="rId10"/>
-    <hyperlink ref="M13" r:id="rId11"/>
-    <hyperlink ref="E14" r:id="rId12"/>
-    <hyperlink ref="M14" r:id="rId13"/>
-    <hyperlink ref="E15" r:id="rId14"/>
-    <hyperlink ref="M15" r:id="rId15"/>
-    <hyperlink ref="M19" r:id="rId16"/>
-    <hyperlink ref="E23" r:id="rId17"/>
-    <hyperlink ref="M23" r:id="rId18"/>
-    <hyperlink ref="E24" r:id="rId19"/>
-    <hyperlink ref="M24" r:id="rId20"/>
-    <hyperlink ref="E25" r:id="rId21"/>
-    <hyperlink ref="M25" r:id="rId22"/>
-    <hyperlink ref="E26" r:id="rId23"/>
-    <hyperlink ref="M26" r:id="rId24"/>
-    <hyperlink ref="E27" r:id="rId25"/>
-    <hyperlink ref="M27" r:id="rId26"/>
-    <hyperlink ref="E28" r:id="rId27"/>
-    <hyperlink ref="M28" r:id="rId28"/>
-    <hyperlink ref="E30" r:id="rId29"/>
-    <hyperlink ref="M30" r:id="rId30"/>
-    <hyperlink ref="E33" r:id="rId31"/>
-    <hyperlink ref="M33" r:id="rId32"/>
-    <hyperlink ref="E34" r:id="rId33"/>
-    <hyperlink ref="M34" r:id="rId34"/>
-    <hyperlink ref="E35" r:id="rId35"/>
-    <hyperlink ref="M35" r:id="rId36"/>
+    <hyperlink ref="E10" r:id="rId6"/>
+    <hyperlink ref="M10" r:id="rId7"/>
+    <hyperlink ref="E11" r:id="rId8"/>
+    <hyperlink ref="M11" r:id="rId9"/>
+    <hyperlink ref="E12" r:id="rId10"/>
+    <hyperlink ref="M12" r:id="rId11"/>
+    <hyperlink ref="E13" r:id="rId12"/>
+    <hyperlink ref="M13" r:id="rId13"/>
+    <hyperlink ref="E14" r:id="rId14"/>
+    <hyperlink ref="M14" r:id="rId15"/>
+    <hyperlink ref="M18" r:id="rId16"/>
+    <hyperlink ref="E22" r:id="rId17"/>
+    <hyperlink ref="M22" r:id="rId18"/>
+    <hyperlink ref="E23" r:id="rId19"/>
+    <hyperlink ref="M23" r:id="rId20"/>
+    <hyperlink ref="E24" r:id="rId21"/>
+    <hyperlink ref="M24" r:id="rId22"/>
+    <hyperlink ref="E25" r:id="rId23"/>
+    <hyperlink ref="M25" r:id="rId24"/>
+    <hyperlink ref="E26" r:id="rId25"/>
+    <hyperlink ref="M26" r:id="rId26"/>
+    <hyperlink ref="E27" r:id="rId27"/>
+    <hyperlink ref="M27" r:id="rId28"/>
+    <hyperlink ref="E29" r:id="rId29"/>
+    <hyperlink ref="M29" r:id="rId30"/>
+    <hyperlink ref="E32" r:id="rId31"/>
+    <hyperlink ref="M32" r:id="rId32"/>
+    <hyperlink ref="E33" r:id="rId33"/>
+    <hyperlink ref="M33" r:id="rId34"/>
+    <hyperlink ref="E34" r:id="rId35"/>
+    <hyperlink ref="M34" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId37"/>

</xml_diff>